<commit_message>
idk what I did but it works
did some shit with the debt_lag1_tgt and we finalize picking the actual model and the variables in it.
</commit_message>
<xml_diff>
--- a/data/processed/CAR_v5_extra_vars.xlsx
+++ b/data/processed/CAR_v5_extra_vars.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AV327"/>
+  <dimension ref="A1:AW327"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -678,6 +678,11 @@
           <t>gdp_lag1_tgt</t>
         </is>
       </c>
+      <c r="AW1" s="1" t="inlineStr">
+        <is>
+          <t>debt_lag1_tgt</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -864,6 +869,9 @@
       <c r="AV2" t="n">
         <v>1.162368267425379</v>
       </c>
+      <c r="AW2" t="n">
+        <v>64.333068764609</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1052,6 +1060,9 @@
       <c r="AV3" t="n">
         <v>1.162368267425379</v>
       </c>
+      <c r="AW3" t="n">
+        <v>64.333068764609</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1242,6 +1253,9 @@
       <c r="AV4" t="n">
         <v>1.474021672511896</v>
       </c>
+      <c r="AW4" t="n">
+        <v>104.74176255873</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1432,6 +1446,9 @@
       <c r="AV5" t="n">
         <v>2.701709209670284</v>
       </c>
+      <c r="AW5" t="n">
+        <v>57.805060845425</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1618,6 +1635,9 @@
       <c r="AV6" t="n">
         <v>2.701709209670284</v>
       </c>
+      <c r="AW6" t="n">
+        <v>57.805060845425</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1806,6 +1826,9 @@
       <c r="AV7" t="n">
         <v>1.162368267425379</v>
       </c>
+      <c r="AW7" t="n">
+        <v>64.333068764609</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1992,6 +2015,9 @@
       <c r="AV8" t="n">
         <v>1.162368267425379</v>
       </c>
+      <c r="AW8" t="n">
+        <v>64.333068764609</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -2178,6 +2204,9 @@
       <c r="AV9" t="n">
         <v>2.45790441131264</v>
       </c>
+      <c r="AW9" t="n">
+        <v>39.801623574722</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -2366,6 +2395,9 @@
       <c r="AV10" t="n">
         <v>2.793176854976991</v>
       </c>
+      <c r="AW10" t="n">
+        <v>48.833793794013</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -2552,6 +2584,9 @@
       <c r="AV11" t="n">
         <v>0.8856972362646189</v>
       </c>
+      <c r="AW11" t="n">
+        <v>66.460091756926</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -2738,6 +2773,9 @@
       <c r="AV12" t="n">
         <v>2.732660761303634</v>
       </c>
+      <c r="AW12" t="n">
+        <v>41.000351027954</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2924,6 +2962,9 @@
       <c r="AV13" t="n">
         <v>2.732660761303634</v>
       </c>
+      <c r="AW13" t="n">
+        <v>41.000351027954</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -3112,6 +3153,9 @@
       <c r="AV14" t="n">
         <v>1.888565802171115</v>
       </c>
+      <c r="AW14" t="n">
+        <v>68.03876765737699</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -3298,6 +3342,9 @@
       <c r="AV15" t="n">
         <v>2.732660761303634</v>
       </c>
+      <c r="AW15" t="n">
+        <v>41.000351027954</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -3484,6 +3531,9 @@
       <c r="AV16" t="n">
         <v>0.8856972362646189</v>
       </c>
+      <c r="AW16" t="n">
+        <v>66.460091756926</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -3670,6 +3720,9 @@
       <c r="AV17" t="n">
         <v>3.551225515372408</v>
       </c>
+      <c r="AW17" t="n">
+        <v>42.39518996425</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -3856,6 +3909,9 @@
       <c r="AV18" t="n">
         <v>2.321737964326417</v>
       </c>
+      <c r="AW18" t="n">
+        <v>95.14187016388399</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -4042,6 +4098,9 @@
       <c r="AV19" t="n">
         <v>2.732660761303634</v>
       </c>
+      <c r="AW19" t="n">
+        <v>41.000351027954</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -4228,6 +4287,9 @@
       <c r="AV20" t="n">
         <v>3.855736152214291</v>
       </c>
+      <c r="AW20" t="n">
+        <v>65.75402484564199</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -4414,6 +4476,9 @@
       <c r="AV21" t="n">
         <v>2.380694024870664</v>
       </c>
+      <c r="AW21" t="n">
+        <v>42.058357189149</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -4602,6 +4667,9 @@
       <c r="AV22" t="n">
         <v>2.380694024870664</v>
       </c>
+      <c r="AW22" t="n">
+        <v>42.058357189149</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -4790,6 +4858,9 @@
       <c r="AV23" t="n">
         <v>4.073628449942746</v>
       </c>
+      <c r="AW23" t="n">
+        <v>48.46713125566</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -4976,6 +5047,9 @@
       <c r="AV24" t="n">
         <v>2.714064517932499</v>
       </c>
+      <c r="AW24" t="n">
+        <v>65.324748897682</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -5162,6 +5236,9 @@
       <c r="AV25" t="n">
         <v>3.855736152214291</v>
       </c>
+      <c r="AW25" t="n">
+        <v>65.75402484564199</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -5350,6 +5427,9 @@
       <c r="AV26" t="n">
         <v>4.073628449942746</v>
       </c>
+      <c r="AW26" t="n">
+        <v>48.46713125566</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -5538,6 +5618,9 @@
       <c r="AV27" t="n">
         <v>4.073628449942746</v>
       </c>
+      <c r="AW27" t="n">
+        <v>48.46713125566</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -5726,6 +5809,9 @@
       <c r="AV28" t="n">
         <v>4.019573228041025</v>
       </c>
+      <c r="AW28" t="n">
+        <v>38.005102365484</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -5912,6 +5998,9 @@
       <c r="AV29" t="n">
         <v>3.855736152214291</v>
       </c>
+      <c r="AW29" t="n">
+        <v>65.75402484564199</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -6096,6 +6185,9 @@
       <c r="AV30" t="n">
         <v>1.799479905207875</v>
       </c>
+      <c r="AW30" t="n">
+        <v>106.25306955972</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -6282,6 +6374,9 @@
       <c r="AV31" t="n">
         <v>4.019573228041025</v>
       </c>
+      <c r="AW31" t="n">
+        <v>38.005102365484</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -6470,6 +6565,9 @@
       <c r="AV32" t="n">
         <v>2.624880019712506</v>
       </c>
+      <c r="AW32" t="n">
+        <v>43.173897815474</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -6658,6 +6756,9 @@
       <c r="AV33" t="n">
         <v>2.624880019712506</v>
       </c>
+      <c r="AW33" t="n">
+        <v>43.173897815474</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -6846,6 +6947,9 @@
       <c r="AV34" t="n">
         <v>2.624880019712506</v>
       </c>
+      <c r="AW34" t="n">
+        <v>43.173897815474</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -7032,6 +7136,9 @@
       <c r="AV35" t="n">
         <v>2.530481861964986</v>
       </c>
+      <c r="AW35" t="n">
+        <v>65.361396134668</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -7218,6 +7325,9 @@
       <c r="AV36" t="n">
         <v>2.914039986071742</v>
       </c>
+      <c r="AW36" t="n">
+        <v>49.515078125596</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -7406,6 +7516,9 @@
       <c r="AV37" t="n">
         <v>2.624880019712506</v>
       </c>
+      <c r="AW37" t="n">
+        <v>43.173897815474</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -7594,6 +7707,9 @@
       <c r="AV38" t="n">
         <v>2.890107189624786</v>
       </c>
+      <c r="AW38" t="n">
+        <v>63.08144063063</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -7780,6 +7896,9 @@
       <c r="AV39" t="n">
         <v>3.885306508388879</v>
       </c>
+      <c r="AW39" t="n">
+        <v>42.741118381438</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -7968,6 +8087,9 @@
       <c r="AV40" t="n">
         <v>3.916375817781798</v>
       </c>
+      <c r="AW40" t="n">
+        <v>44.751849868379</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -8154,6 +8276,9 @@
       <c r="AV41" t="n">
         <v>3.224911317116664</v>
       </c>
+      <c r="AW41" t="n">
+        <v>39.072554361199</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -8342,6 +8467,9 @@
       <c r="AV42" t="n">
         <v>2.890107189624786</v>
       </c>
+      <c r="AW42" t="n">
+        <v>63.08144063063</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -8530,6 +8658,9 @@
       <c r="AV43" t="n">
         <v>3.916375817781798</v>
       </c>
+      <c r="AW43" t="n">
+        <v>44.751849868379</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -8716,6 +8847,9 @@
       <c r="AV44" t="n">
         <v>3.676924838925231</v>
       </c>
+      <c r="AW44" t="n">
+        <v>87.32462407492</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -8902,6 +9036,9 @@
       <c r="AV45" t="n">
         <v>0.4469049477175275</v>
       </c>
+      <c r="AW45" t="n">
+        <v>93.16004344093101</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -9088,6 +9225,9 @@
       <c r="AV46" t="n">
         <v>0.9104031961453529</v>
       </c>
+      <c r="AW46" t="n">
+        <v>64.586203700843</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -9277,6 +9417,9 @@
       <c r="AV47" t="n">
         <v>-0.2487972981322457</v>
       </c>
+      <c r="AW47" t="n">
+        <v>50.827371987952</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -9463,6 +9606,9 @@
       <c r="AV48" t="n">
         <v>-1.02313847687941</v>
       </c>
+      <c r="AW48" t="n">
+        <v>105.78767746274</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -9649,6 +9795,9 @@
       <c r="AV49" t="n">
         <v>-1.02313847687941</v>
       </c>
+      <c r="AW49" t="n">
+        <v>105.78767746274</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -9835,6 +9984,9 @@
       <c r="AV50" t="n">
         <v>0.4469049477175275</v>
       </c>
+      <c r="AW50" t="n">
+        <v>93.16004344093101</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -10039,6 +10191,9 @@
       <c r="AV51" t="n">
         <v>-0.9231230829503119</v>
       </c>
+      <c r="AW51" t="n">
+        <v>37.735727790621</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -10227,6 +10382,9 @@
       <c r="AV52" t="n">
         <v>-1.02313847687941</v>
       </c>
+      <c r="AW52" t="n">
+        <v>105.78767746274</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -10415,6 +10573,9 @@
       <c r="AV53" t="n">
         <v>0.7844312192730314</v>
       </c>
+      <c r="AW53" t="n">
+        <v>32.562688864522</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -10603,6 +10764,9 @@
       <c r="AV54" t="n">
         <v>-0.2487972981322457</v>
       </c>
+      <c r="AW54" t="n">
+        <v>50.827371987952</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -10789,6 +10953,9 @@
       <c r="AV55" t="n">
         <v>0.4469049477175275</v>
       </c>
+      <c r="AW55" t="n">
+        <v>93.16004344093101</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -10977,6 +11144,9 @@
       <c r="AV56" t="n">
         <v>0.3801714255223629</v>
       </c>
+      <c r="AW56" t="n">
+        <v>69.735692990293</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -11165,6 +11335,9 @@
       <c r="AV57" t="n">
         <v>-0.9231230829503119</v>
       </c>
+      <c r="AW57" t="n">
+        <v>37.735727790621</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -11351,6 +11524,9 @@
       <c r="AV58" t="n">
         <v>0.3801714255223629</v>
       </c>
+      <c r="AW58" t="n">
+        <v>69.735692990293</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -11539,6 +11715,9 @@
       <c r="AV59" t="n">
         <v>-1.02313847687941</v>
       </c>
+      <c r="AW59" t="n">
+        <v>105.78767746274</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -11725,6 +11904,9 @@
       <c r="AV60" t="n">
         <v>-2.297374630715453</v>
       </c>
+      <c r="AW60" t="n">
+        <v>43.087987059163</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -11913,6 +12095,9 @@
       <c r="AV61" t="n">
         <v>-5.545164537717056</v>
       </c>
+      <c r="AW61" t="n">
+        <v>71.71568057654299</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -12101,6 +12286,9 @@
       <c r="AV62" t="n">
         <v>-2.824551502889619</v>
       </c>
+      <c r="AW62" t="n">
+        <v>84.03127004341</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -12289,6 +12477,9 @@
       <c r="AV63" t="n">
         <v>-5.305154032510998</v>
       </c>
+      <c r="AW63" t="n">
+        <v>116.12127583182</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -12477,6 +12668,9 @@
       <c r="AV64" t="n">
         <v>-4.620553719568605</v>
       </c>
+      <c r="AW64" t="n">
+        <v>64.91501173164799</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -12665,6 +12859,9 @@
       <c r="AV65" t="n">
         <v>-3.665290445065949</v>
       </c>
+      <c r="AW65" t="n">
+        <v>56.289780742748</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -12853,6 +13050,9 @@
       <c r="AV66" t="n">
         <v>-4.255573742711448</v>
       </c>
+      <c r="AW66" t="n">
+        <v>40.947598349172</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -13041,6 +13241,9 @@
       <c r="AV67" t="n">
         <v>-2.297374630715453</v>
       </c>
+      <c r="AW67" t="n">
+        <v>43.087987059163</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -13229,6 +13432,9 @@
       <c r="AV68" t="n">
         <v>-5.545164537717056</v>
       </c>
+      <c r="AW68" t="n">
+        <v>71.71568057654299</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -13415,6 +13621,9 @@
       <c r="AV69" t="n">
         <v>-5.545164537717056</v>
       </c>
+      <c r="AW69" t="n">
+        <v>71.71568057654299</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -13601,6 +13810,9 @@
       <c r="AV70" t="n">
         <v>-4.255573742711448</v>
       </c>
+      <c r="AW70" t="n">
+        <v>40.947598349172</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -13789,6 +14001,9 @@
       <c r="AV71" t="n">
         <v>-4.620553719568605</v>
       </c>
+      <c r="AW71" t="n">
+        <v>64.91501173164799</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -13975,6 +14190,9 @@
       <c r="AV72" t="n">
         <v>4.146767545324366</v>
       </c>
+      <c r="AW72" t="n">
+        <v>80.37552655520101</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -14163,6 +14381,9 @@
       <c r="AV73" t="n">
         <v>2.233315126310799</v>
       </c>
+      <c r="AW73" t="n">
+        <v>75.86022965982499</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -14351,6 +14572,9 @@
       <c r="AV74" t="n">
         <v>2.233315126310799</v>
       </c>
+      <c r="AW74" t="n">
+        <v>75.86022965982499</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -14537,6 +14761,9 @@
       <c r="AV75" t="n">
         <v>4.146767545324366</v>
       </c>
+      <c r="AW75" t="n">
+        <v>80.37552655520101</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -14723,6 +14950,9 @@
       <c r="AV76" t="n">
         <v>4.146767545324366</v>
       </c>
+      <c r="AW76" t="n">
+        <v>80.37552655520101</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -14911,6 +15141,9 @@
       <c r="AV77" t="n">
         <v>5.750735843227247</v>
       </c>
+      <c r="AW77" t="n">
+        <v>38.301932321582</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -15099,6 +15332,9 @@
       <c r="AV78" t="n">
         <v>1.682972350562579</v>
       </c>
+      <c r="AW78" t="n">
+        <v>86.13499277379</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -15287,6 +15523,9 @@
       <c r="AV79" t="n">
         <v>2.000324726999807</v>
       </c>
+      <c r="AW79" t="n">
+        <v>86.31331100407</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -15473,6 +15712,9 @@
       <c r="AV80" t="n">
         <v>4.146767545324366</v>
       </c>
+      <c r="AW80" t="n">
+        <v>80.37552655520101</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -15661,6 +15903,9 @@
       <c r="AV81" t="n">
         <v>1.682972350562579</v>
       </c>
+      <c r="AW81" t="n">
+        <v>86.13499277379</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -15849,6 +16094,9 @@
       <c r="AV82" t="n">
         <v>4.146767545324366</v>
       </c>
+      <c r="AW82" t="n">
+        <v>80.37552655520101</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -16035,6 +16283,9 @@
       <c r="AV83" t="n">
         <v>4.146767545324366</v>
       </c>
+      <c r="AW83" t="n">
+        <v>80.37552655520101</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -16221,6 +16472,9 @@
       <c r="AV84" t="n">
         <v>1.773345206572458</v>
       </c>
+      <c r="AW84" t="n">
+        <v>61.166928094413</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -16409,6 +16663,9 @@
       <c r="AV85" t="n">
         <v>1.138362347448933</v>
       </c>
+      <c r="AW85" t="n">
+        <v>81.42506571072801</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -16597,6 +16854,9 @@
       <c r="AV86" t="n">
         <v>1.138362347448933</v>
       </c>
+      <c r="AW86" t="n">
+        <v>81.42506571072801</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -16785,6 +17045,9 @@
       <c r="AV87" t="n">
         <v>3.163910481452035</v>
       </c>
+      <c r="AW87" t="n">
+        <v>37.380423149749</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -16971,6 +17234,9 @@
       <c r="AV88" t="n">
         <v>3.757968865863475</v>
       </c>
+      <c r="AW88" t="n">
+        <v>77.84923266164699</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -17159,6 +17425,9 @@
       <c r="AV89" t="n">
         <v>3.757968865863475</v>
       </c>
+      <c r="AW89" t="n">
+        <v>77.84923266164699</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -17347,6 +17616,9 @@
       <c r="AV90" t="n">
         <v>3.163910481452035</v>
       </c>
+      <c r="AW90" t="n">
+        <v>37.380423149749</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -17535,6 +17807,9 @@
       <c r="AV91" t="n">
         <v>3.163910481452035</v>
       </c>
+      <c r="AW91" t="n">
+        <v>37.380423149749</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -17723,6 +17998,9 @@
       <c r="AV92" t="n">
         <v>1.138362347448933</v>
       </c>
+      <c r="AW92" t="n">
+        <v>81.42506571072801</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -17909,6 +18187,9 @@
       <c r="AV93" t="n">
         <v>2.437576568770794</v>
       </c>
+      <c r="AW93" t="n">
+        <v>88.91020026049701</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -18095,6 +18376,9 @@
       <c r="AV94" t="n">
         <v>1.138362347448933</v>
       </c>
+      <c r="AW94" t="n">
+        <v>81.42506571072801</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -18283,6 +18567,9 @@
       <c r="AV95" t="n">
         <v>0.4742913058555445</v>
       </c>
+      <c r="AW95" t="n">
+        <v>79.157292938815</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -18469,6 +18756,9 @@
       <c r="AV96" t="n">
         <v>1.50899837441014</v>
       </c>
+      <c r="AW96" t="n">
+        <v>84.48260066580499</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -18655,6 +18945,9 @@
       <c r="AV97" t="n">
         <v>-2.865113672910695</v>
       </c>
+      <c r="AW97" t="n">
+        <v>89.560379607786</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -18843,6 +19136,9 @@
       <c r="AV98" t="n">
         <v>-3.125238795438165</v>
       </c>
+      <c r="AW98" t="n">
+        <v>125.87049589393</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -19031,6 +19327,9 @@
       <c r="AV99" t="n">
         <v>1.50899837441014</v>
       </c>
+      <c r="AW99" t="n">
+        <v>84.48260066580499</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -19217,6 +19516,9 @@
       <c r="AV100" t="n">
         <v>0.4742913058555445</v>
       </c>
+      <c r="AW100" t="n">
+        <v>79.157292938815</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -19403,6 +19705,9 @@
       <c r="AV101" t="n">
         <v>1.179253833251082</v>
       </c>
+      <c r="AW101" t="n">
+        <v>42.569499885418</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -19589,6 +19894,9 @@
       <c r="AV102" t="n">
         <v>-0.4144657210708829</v>
       </c>
+      <c r="AW102" t="n">
+        <v>37.686333135724</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -19777,6 +20085,9 @@
       <c r="AV103" t="n">
         <v>-0.3989599645054511</v>
       </c>
+      <c r="AW103" t="n">
+        <v>118.72991735163</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -19965,6 +20276,9 @@
       <c r="AV104" t="n">
         <v>1.50899837441014</v>
       </c>
+      <c r="AW104" t="n">
+        <v>84.48260066580499</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -20151,6 +20465,9 @@
       <c r="AV105" t="n">
         <v>0.7817564459134019</v>
       </c>
+      <c r="AW105" t="n">
+        <v>94.686825462051</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -20337,6 +20654,9 @@
       <c r="AV106" t="n">
         <v>1.799921493626627</v>
       </c>
+      <c r="AW106" t="n">
+        <v>85.316058901031</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -20523,6 +20843,9 @@
       <c r="AV107" t="n">
         <v>1.792144057074836</v>
       </c>
+      <c r="AW107" t="n">
+        <v>41.945930095193</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -20709,6 +21032,9 @@
       <c r="AV108" t="n">
         <v>-1.818025061042832</v>
       </c>
+      <c r="AW108" t="n">
+        <v>131.81630273306</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -20895,6 +21221,9 @@
       <c r="AV109" t="n">
         <v>-1.427322191818803</v>
       </c>
+      <c r="AW109" t="n">
+        <v>100.00031287415</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -21099,6 +21428,9 @@
       <c r="AV110" t="n">
         <v>0.386224576109953</v>
       </c>
+      <c r="AW110" t="n">
+        <v>76.794662537318</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -21285,6 +21617,9 @@
       <c r="AV111" t="n">
         <v>1.392673470172952</v>
       </c>
+      <c r="AW111" t="n">
+        <v>43.911826885918</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -21473,6 +21808,9 @@
       <c r="AV112" t="n">
         <v>0.3054944785623803</v>
       </c>
+      <c r="AW112" t="n">
+        <v>105.48564447159</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -21661,6 +21999,9 @@
       <c r="AV113" t="n">
         <v>0.7817564459134019</v>
       </c>
+      <c r="AW113" t="n">
+        <v>94.686825462051</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -21849,6 +22190,9 @@
       <c r="AV114" t="n">
         <v>2.295763808728395</v>
       </c>
+      <c r="AW114" t="n">
+        <v>45.20099109843</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -22035,6 +22379,9 @@
       <c r="AV115" t="n">
         <v>2.349881275086261</v>
       </c>
+      <c r="AW115" t="n">
+        <v>42.06696758215</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -22221,6 +22568,9 @@
       <c r="AV116" t="n">
         <v>1.520485922798187</v>
       </c>
+      <c r="AW116" t="n">
+        <v>104.41761636038</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -22409,6 +22759,9 @@
       <c r="AV117" t="n">
         <v>1.612610074491229</v>
       </c>
+      <c r="AW117" t="n">
+        <v>67.16590999179201</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -22595,6 +22948,9 @@
       <c r="AV118" t="n">
         <v>3.194637312802101</v>
       </c>
+      <c r="AW118" t="n">
+        <v>87.094325197019</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -22781,6 +23137,9 @@
       <c r="AV119" t="n">
         <v>2.169498928790787</v>
       </c>
+      <c r="AW119" t="n">
+        <v>73.823031854132</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -22969,6 +23328,9 @@
       <c r="AV120" t="n">
         <v>3.194637312802101</v>
       </c>
+      <c r="AW120" t="n">
+        <v>87.094325197019</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -23155,6 +23517,9 @@
       <c r="AV121" t="n">
         <v>2.169498928790787</v>
       </c>
+      <c r="AW121" t="n">
+        <v>73.823031854132</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -23343,6 +23708,9 @@
       <c r="AV122" t="n">
         <v>9.336033728686232</v>
       </c>
+      <c r="AW122" t="n">
+        <v>101.27607447502</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -23529,6 +23897,9 @@
       <c r="AV123" t="n">
         <v>3.194637312802101</v>
       </c>
+      <c r="AW123" t="n">
+        <v>87.094325197019</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -23715,6 +24086,9 @@
       <c r="AV124" t="n">
         <v>1.277999793806444</v>
       </c>
+      <c r="AW124" t="n">
+        <v>44.290452475481</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -23903,6 +24277,9 @@
       <c r="AV125" t="n">
         <v>2.349881275086261</v>
       </c>
+      <c r="AW125" t="n">
+        <v>42.06696758215</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -24091,6 +24468,9 @@
       <c r="AV126" t="n">
         <v>3.194637312802101</v>
       </c>
+      <c r="AW126" t="n">
+        <v>87.094325197019</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -24280,6 +24660,9 @@
       <c r="AV127" t="n">
         <v>2.349881275086261</v>
       </c>
+      <c r="AW127" t="n">
+        <v>42.06696758215</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -24468,6 +24851,9 @@
       <c r="AV128" t="n">
         <v>2.295763808728395</v>
       </c>
+      <c r="AW128" t="n">
+        <v>45.20099109843</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -24654,6 +25040,9 @@
       <c r="AV129" t="n">
         <v>1.612610074491229</v>
       </c>
+      <c r="AW129" t="n">
+        <v>67.16590999179201</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -24842,6 +25231,9 @@
       <c r="AV130" t="n">
         <v>1.066754734889088</v>
       </c>
+      <c r="AW130" t="n">
+        <v>97.0737325512</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -25030,6 +25422,9 @@
       <c r="AV131" t="n">
         <v>2.222888449084365</v>
       </c>
+      <c r="AW131" t="n">
+        <v>87.86668691242301</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -25216,6 +25611,9 @@
       <c r="AV132" t="n">
         <v>4.410140675793414</v>
       </c>
+      <c r="AW132" t="n">
+        <v>44.035592881896</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -25402,6 +25800,9 @@
       <c r="AV133" t="n">
         <v>2.104414587125873</v>
       </c>
+      <c r="AW133" t="n">
+        <v>39.894178226249</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -25588,6 +25989,9 @@
       <c r="AV134" t="n">
         <v>4.060866697185688</v>
       </c>
+      <c r="AW134" t="n">
+        <v>102.44212445452</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -25776,6 +26180,9 @@
       <c r="AV135" t="n">
         <v>4.410140675793414</v>
       </c>
+      <c r="AW135" t="n">
+        <v>44.035592881896</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -25962,6 +26369,9 @@
       <c r="AV136" t="n">
         <v>2.120605224217172</v>
       </c>
+      <c r="AW136" t="n">
+        <v>63.799334930454</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -26150,6 +26560,9 @@
       <c r="AV137" t="n">
         <v>1.066754734889088</v>
       </c>
+      <c r="AW137" t="n">
+        <v>97.0737325512</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -26338,6 +26751,9 @@
       <c r="AV138" t="n">
         <v>2.222888449084365</v>
       </c>
+      <c r="AW138" t="n">
+        <v>87.86668691242301</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -26524,6 +26940,9 @@
       <c r="AV139" t="n">
         <v>4.060866697185688</v>
       </c>
+      <c r="AW139" t="n">
+        <v>102.44212445452</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -26710,6 +27129,9 @@
       <c r="AV140" t="n">
         <v>1.652719771746277</v>
       </c>
+      <c r="AW140" t="n">
+        <v>70.559882034579</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -26898,6 +27320,9 @@
       <c r="AV141" t="n">
         <v>4.060866697185688</v>
       </c>
+      <c r="AW141" t="n">
+        <v>102.44212445452</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -27086,6 +27511,9 @@
       <c r="AV142" t="n">
         <v>4.410140675793414</v>
       </c>
+      <c r="AW142" t="n">
+        <v>44.035592881896</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -27274,6 +27702,9 @@
       <c r="AV143" t="n">
         <v>1.47416438588013</v>
       </c>
+      <c r="AW143" t="n">
+        <v>105.23035646577</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -27462,6 +27893,9 @@
       <c r="AV144" t="n">
         <v>4.410140675793414</v>
       </c>
+      <c r="AW144" t="n">
+        <v>44.035592881896</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -27650,6 +28084,9 @@
       <c r="AV145" t="n">
         <v>2.222888449084365</v>
       </c>
+      <c r="AW145" t="n">
+        <v>87.86668691242301</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -27836,6 +28273,9 @@
       <c r="AV146" t="n">
         <v>2.222888449084365</v>
       </c>
+      <c r="AW146" t="n">
+        <v>87.86668691242301</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -28022,6 +28462,9 @@
       <c r="AV147" t="n">
         <v>2.004141093604872</v>
       </c>
+      <c r="AW147" t="n">
+        <v>131.5057445501</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -28210,6 +28653,9 @@
       <c r="AV148" t="n">
         <v>2.349740804325393</v>
       </c>
+      <c r="AW148" t="n">
+        <v>42.373485372264</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -28396,6 +28842,9 @@
       <c r="AV149" t="n">
         <v>2.349740804325393</v>
       </c>
+      <c r="AW149" t="n">
+        <v>42.373485372264</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -28582,6 +29031,9 @@
       <c r="AV150" t="n">
         <v>2.294710676842811</v>
       </c>
+      <c r="AW150" t="n">
+        <v>67.630651010134</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -28771,6 +29223,9 @@
       <c r="AV151" t="n">
         <v>3.073045474798548</v>
       </c>
+      <c r="AW151" t="n">
+        <v>37.304314351367</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -28959,6 +29414,9 @@
       <c r="AV152" t="n">
         <v>2.349740804325393</v>
       </c>
+      <c r="AW152" t="n">
+        <v>42.373485372264</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -29145,6 +29603,9 @@
       <c r="AV153" t="n">
         <v>1.236221107275099</v>
       </c>
+      <c r="AW153" t="n">
+        <v>134.19551269697</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -29331,6 +29792,9 @@
       <c r="AV154" t="n">
         <v>2.117219670961077</v>
       </c>
+      <c r="AW154" t="n">
+        <v>82.84042862575799</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -29517,6 +29981,9 @@
       <c r="AV155" t="n">
         <v>2.349740804325393</v>
       </c>
+      <c r="AW155" t="n">
+        <v>42.373485372264</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -29705,6 +30172,9 @@
       <c r="AV156" t="n">
         <v>0.860031082016107</v>
       </c>
+      <c r="AW156" t="n">
+        <v>98.024778336434</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -29891,6 +30361,9 @@
       <c r="AV157" t="n">
         <v>1.193502639951106</v>
       </c>
+      <c r="AW157" t="n">
+        <v>105.00714974947</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -30079,6 +30552,9 @@
       <c r="AV158" t="n">
         <v>1.921710077638309</v>
       </c>
+      <c r="AW158" t="n">
+        <v>87.82518973009699</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -30267,6 +30743,9 @@
       <c r="AV159" t="n">
         <v>2.294710676842811</v>
       </c>
+      <c r="AW159" t="n">
+        <v>67.630651010134</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -30453,6 +30932,9 @@
       <c r="AV160" t="n">
         <v>2.294710676842811</v>
       </c>
+      <c r="AW160" t="n">
+        <v>67.630651010134</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -30641,6 +31123,9 @@
       <c r="AV161" t="n">
         <v>2.915156028081739</v>
       </c>
+      <c r="AW161" t="n">
+        <v>101.96650275565</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -30827,6 +31312,9 @@
       <c r="AV162" t="n">
         <v>1.193502639951106</v>
       </c>
+      <c r="AW162" t="n">
+        <v>105.00714974947</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -31013,6 +31501,9 @@
       <c r="AV163" t="n">
         <v>2.068689667099605</v>
       </c>
+      <c r="AW163" t="n">
+        <v>40.936561690762</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -31201,6 +31692,9 @@
       <c r="AV164" t="n">
         <v>0.860031082016107</v>
       </c>
+      <c r="AW164" t="n">
+        <v>98.024778336434</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -31387,6 +31881,9 @@
       <c r="AV165" t="n">
         <v>2.004141093604872</v>
       </c>
+      <c r="AW165" t="n">
+        <v>131.5057445501</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -31573,6 +32070,9 @@
       <c r="AV166" t="n">
         <v>1.474467656530919</v>
       </c>
+      <c r="AW166" t="n">
+        <v>102.0217953039</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -31761,6 +32261,9 @@
       <c r="AV167" t="n">
         <v>2.896042080816301</v>
       </c>
+      <c r="AW167" t="n">
+        <v>101.14423857972</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -31947,6 +32450,9 @@
       <c r="AV168" t="n">
         <v>1.603699946483616</v>
       </c>
+      <c r="AW168" t="n">
+        <v>133.68902882039</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -32135,6 +32641,9 @@
       <c r="AV169" t="n">
         <v>2.716024519315923</v>
       </c>
+      <c r="AW169" t="n">
+        <v>63.952376234949</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -32321,6 +32830,9 @@
       <c r="AV170" t="n">
         <v>3.303370161133216</v>
       </c>
+      <c r="AW170" t="n">
+        <v>66.512105153767</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -32507,6 +33019,9 @@
       <c r="AV171" t="n">
         <v>1.603699946483616</v>
       </c>
+      <c r="AW171" t="n">
+        <v>133.68902882039</v>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -32693,6 +33208,9 @@
       <c r="AV172" t="n">
         <v>2.716024519315923</v>
       </c>
+      <c r="AW172" t="n">
+        <v>63.952376234949</v>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -32881,6 +33399,9 @@
       <c r="AV173" t="n">
         <v>2.083614850620762</v>
       </c>
+      <c r="AW173" t="n">
+        <v>98.48331172771501</v>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -33067,6 +33588,9 @@
       <c r="AV174" t="n">
         <v>1.362799557114158</v>
       </c>
+      <c r="AW174" t="n">
+        <v>41.753380143385</v>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -33253,6 +33777,9 @@
       <c r="AV175" t="n">
         <v>2.896042080816301</v>
       </c>
+      <c r="AW175" t="n">
+        <v>101.14423857972</v>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -33441,6 +33968,9 @@
       <c r="AV176" t="n">
         <v>2.656504893099722</v>
       </c>
+      <c r="AW176" t="n">
+        <v>86.72315054824</v>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -33627,6 +34157,9 @@
       <c r="AV177" t="n">
         <v>2.656504893099722</v>
       </c>
+      <c r="AW177" t="n">
+        <v>86.72315054824</v>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -33815,6 +34348,9 @@
       <c r="AV178" t="n">
         <v>1.825156014947169</v>
       </c>
+      <c r="AW178" t="n">
+        <v>41.105350817723</v>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -34003,6 +34539,9 @@
       <c r="AV179" t="n">
         <v>2.716024519315923</v>
       </c>
+      <c r="AW179" t="n">
+        <v>63.952376234949</v>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -34187,6 +34726,9 @@
       <c r="AV180" t="n">
         <v>3.303370161133216</v>
       </c>
+      <c r="AW180" t="n">
+        <v>66.512105153767</v>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -34373,6 +34915,9 @@
       <c r="AV181" t="n">
         <v>1.192977729885044</v>
       </c>
+      <c r="AW181" t="n">
+        <v>65.2783212983</v>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -34559,6 +35104,9 @@
       <c r="AV182" t="n">
         <v>2.258740396249522</v>
       </c>
+      <c r="AW182" t="n">
+        <v>51.557591839171</v>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -34745,6 +35293,9 @@
       <c r="AV183" t="n">
         <v>2.395411203642468</v>
       </c>
+      <c r="AW183" t="n">
+        <v>99.718282717797</v>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -34933,6 +35484,9 @@
       <c r="AV184" t="n">
         <v>1.116443109262249</v>
       </c>
+      <c r="AW184" t="n">
+        <v>60.728535497052</v>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -35121,6 +35675,9 @@
       <c r="AV185" t="n">
         <v>2.860445794616325</v>
       </c>
+      <c r="AW185" t="n">
+        <v>39.7840016917</v>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -35307,6 +35864,9 @@
       <c r="AV186" t="n">
         <v>1.405190266092731</v>
       </c>
+      <c r="AW186" t="n">
+        <v>86.34546978493699</v>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -35493,6 +36053,9 @@
       <c r="AV187" t="n">
         <v>1.192977729885044</v>
       </c>
+      <c r="AW187" t="n">
+        <v>65.2783212983</v>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -35681,6 +36244,9 @@
       <c r="AV188" t="n">
         <v>1.405190266092731</v>
       </c>
+      <c r="AW188" t="n">
+        <v>86.34546978493699</v>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -35869,6 +36435,9 @@
       <c r="AV189" t="n">
         <v>1.405190266092731</v>
       </c>
+      <c r="AW189" t="n">
+        <v>86.34546978493699</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -36057,6 +36626,9 @@
       <c r="AV190" t="n">
         <v>2.860445794616325</v>
       </c>
+      <c r="AW190" t="n">
+        <v>39.7840016917</v>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -36245,6 +36817,9 @@
       <c r="AV191" t="n">
         <v>2.860445794616325</v>
       </c>
+      <c r="AW191" t="n">
+        <v>39.7840016917</v>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -36431,6 +37006,9 @@
       <c r="AV192" t="n">
         <v>2.395411203642468</v>
       </c>
+      <c r="AW192" t="n">
+        <v>99.718282717797</v>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -36619,6 +37197,9 @@
       <c r="AV193" t="n">
         <v>1.405190266092731</v>
       </c>
+      <c r="AW193" t="n">
+        <v>86.34546978493699</v>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -36807,6 +37388,9 @@
       <c r="AV194" t="n">
         <v>1.64590872932709</v>
       </c>
+      <c r="AW194" t="n">
+        <v>98.159104237877</v>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -36995,6 +37579,9 @@
       <c r="AV195" t="n">
         <v>1.64590872932709</v>
       </c>
+      <c r="AW195" t="n">
+        <v>98.159104237877</v>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -37183,6 +37770,9 @@
       <c r="AV196" t="n">
         <v>1.405190266092731</v>
       </c>
+      <c r="AW196" t="n">
+        <v>86.34546978493699</v>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -37369,6 +37959,9 @@
       <c r="AV197" t="n">
         <v>0.4291625343719119</v>
       </c>
+      <c r="AW197" t="n">
+        <v>133.82273913912</v>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -37557,6 +38150,9 @@
       <c r="AV198" t="n">
         <v>1.349738438261227</v>
       </c>
+      <c r="AW198" t="n">
+        <v>65.241487437771</v>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -37743,6 +38339,9 @@
       <c r="AV199" t="n">
         <v>0.9878933491675781</v>
       </c>
+      <c r="AW199" t="n">
+        <v>58.556132032771</v>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -37929,6 +38528,9 @@
       <c r="AV200" t="n">
         <v>2.027446476396349</v>
       </c>
+      <c r="AW200" t="n">
+        <v>97.88586068053699</v>
+      </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -38117,6 +38719,9 @@
       <c r="AV201" t="n">
         <v>2.549647852530484</v>
       </c>
+      <c r="AW201" t="n">
+        <v>35.695844772654</v>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -38305,6 +38910,9 @@
       <c r="AV202" t="n">
         <v>1.624475159475324</v>
       </c>
+      <c r="AW202" t="n">
+        <v>85.65750534598099</v>
+      </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -38493,6 +39101,9 @@
       <c r="AV203" t="n">
         <v>0.9878933491675781</v>
       </c>
+      <c r="AW203" t="n">
+        <v>58.556132032771</v>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -38681,6 +39292,9 @@
       <c r="AV204" t="n">
         <v>1.349738438261227</v>
       </c>
+      <c r="AW204" t="n">
+        <v>65.241487437771</v>
+      </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
@@ -38869,6 +39483,9 @@
       <c r="AV205" t="n">
         <v>1.624475159475324</v>
       </c>
+      <c r="AW205" t="n">
+        <v>85.65750534598099</v>
+      </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
@@ -39055,6 +39672,9 @@
       <c r="AV206" t="n">
         <v>2.027446476396349</v>
       </c>
+      <c r="AW206" t="n">
+        <v>97.88586068053699</v>
+      </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -39241,6 +39861,9 @@
       <c r="AV207" t="n">
         <v>0.9878933491675781</v>
       </c>
+      <c r="AW207" t="n">
+        <v>58.556132032771</v>
+      </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
@@ -39427,6 +40050,9 @@
       <c r="AV208" t="n">
         <v>1.624475159475324</v>
       </c>
+      <c r="AW208" t="n">
+        <v>85.65750534598099</v>
+      </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
@@ -39613,6 +40239,9 @@
       <c r="AV209" t="n">
         <v>0.9878933491675781</v>
       </c>
+      <c r="AW209" t="n">
+        <v>58.556132032771</v>
+      </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
@@ -39799,6 +40428,9 @@
       <c r="AV210" t="n">
         <v>5.040550288017997</v>
       </c>
+      <c r="AW210" t="n">
+        <v>55.924328040146</v>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
@@ -39987,6 +40619,9 @@
       <c r="AV211" t="n">
         <v>0.9878933491675781</v>
       </c>
+      <c r="AW211" t="n">
+        <v>58.556132032771</v>
+      </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
@@ -40175,6 +40810,9 @@
       <c r="AV212" t="n">
         <v>1.961178531513497</v>
       </c>
+      <c r="AW212" t="n">
+        <v>97.57881607389299</v>
+      </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
@@ -40363,6 +41001,9 @@
       <c r="AV213" t="n">
         <v>2.549647852530484</v>
       </c>
+      <c r="AW213" t="n">
+        <v>35.695844772654</v>
+      </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
@@ -40551,6 +41192,9 @@
       <c r="AV214" t="n">
         <v>1.624475159475324</v>
       </c>
+      <c r="AW214" t="n">
+        <v>85.65750534598099</v>
+      </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
@@ -40739,6 +41383,9 @@
       <c r="AV215" t="n">
         <v>2.549647852530484</v>
       </c>
+      <c r="AW215" t="n">
+        <v>35.695844772654</v>
+      </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
@@ -40927,6 +41574,9 @@
       <c r="AV216" t="n">
         <v>2.549647852530484</v>
       </c>
+      <c r="AW216" t="n">
+        <v>35.695844772654</v>
+      </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
@@ -41115,6 +41765,9 @@
       <c r="AV217" t="n">
         <v>2.300091594761966</v>
       </c>
+      <c r="AW217" t="n">
+        <v>47.582634643219</v>
+      </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
@@ -41303,6 +41956,9 @@
       <c r="AV218" t="n">
         <v>1.624475159475324</v>
       </c>
+      <c r="AW218" t="n">
+        <v>85.65750534598099</v>
+      </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -41491,6 +42147,9 @@
       <c r="AV219" t="n">
         <v>0.9878933491675781</v>
       </c>
+      <c r="AW219" t="n">
+        <v>58.556132032771</v>
+      </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
@@ -41695,6 +42354,9 @@
       <c r="AV220" t="n">
         <v>-4.095137490646891</v>
       </c>
+      <c r="AW220" t="n">
+        <v>67.858169885379</v>
+      </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
@@ -41883,6 +42545,9 @@
       <c r="AV221" t="n">
         <v>-10.2969188737567</v>
       </c>
+      <c r="AW221" t="n">
+        <v>105.80010911054</v>
+      </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
@@ -42070,6 +42735,9 @@
       <c r="AV222" t="n">
         <v>-2.491036209772389</v>
       </c>
+      <c r="AW222" t="n">
+        <v>75.26035315259401</v>
+      </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
@@ -42256,6 +42924,9 @@
       <c r="AV223" t="n">
         <v>-4.095137490646891</v>
       </c>
+      <c r="AW223" t="n">
+        <v>67.858169885379</v>
+      </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
@@ -42442,6 +43113,9 @@
       <c r="AV224" t="n">
         <v>-7.44064593044142</v>
       </c>
+      <c r="AW224" t="n">
+        <v>114.8530178201</v>
+      </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
@@ -42630,6 +43304,9 @@
       <c r="AV225" t="n">
         <v>-7.44064593044142</v>
       </c>
+      <c r="AW225" t="n">
+        <v>114.8530178201</v>
+      </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
@@ -42834,6 +43511,9 @@
       <c r="AV226" t="n">
         <v>-2.141737206500537</v>
       </c>
+      <c r="AW226" t="n">
+        <v>43.198776482207</v>
+      </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
@@ -43020,6 +43700,9 @@
       <c r="AV227" t="n">
         <v>-4.095137490646891</v>
       </c>
+      <c r="AW227" t="n">
+        <v>67.858169885379</v>
+      </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
@@ -43208,6 +43891,9 @@
       <c r="AV228" t="n">
         <v>-2.005337503537632</v>
       </c>
+      <c r="AW228" t="n">
+        <v>40.311887445036</v>
+      </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
@@ -43395,6 +44081,9 @@
       <c r="AV229" t="n">
         <v>-4.095137490646891</v>
       </c>
+      <c r="AW229" t="n">
+        <v>67.858169885379</v>
+      </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
@@ -43583,6 +44272,9 @@
       <c r="AV230" t="n">
         <v>-7.44064593044142</v>
       </c>
+      <c r="AW230" t="n">
+        <v>114.8530178201</v>
+      </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
@@ -43769,6 +44461,9 @@
       <c r="AV231" t="n">
         <v>-4.095137490646891</v>
       </c>
+      <c r="AW231" t="n">
+        <v>67.858169885379</v>
+      </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
@@ -43973,6 +44668,9 @@
       <c r="AV232" t="n">
         <v>-4.095137490646891</v>
       </c>
+      <c r="AW232" t="n">
+        <v>67.858169885379</v>
+      </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
@@ -44161,6 +44859,9 @@
       <c r="AV233" t="n">
         <v>-10.2969188737567</v>
       </c>
+      <c r="AW233" t="n">
+        <v>105.80010911054</v>
+      </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
@@ -44349,6 +45050,9 @@
       <c r="AV234" t="n">
         <v>7.157898830572094</v>
       </c>
+      <c r="AW234" t="n">
+        <v>57.007189840034</v>
+      </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
@@ -44537,6 +45241,9 @@
       <c r="AV235" t="n">
         <v>-2.141737206500537</v>
       </c>
+      <c r="AW235" t="n">
+        <v>43.198776482207</v>
+      </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
@@ -44723,6 +45430,9 @@
       <c r="AV236" t="n">
         <v>-10.94007065918665</v>
       </c>
+      <c r="AW236" t="n">
+        <v>119.17898068922</v>
+      </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
@@ -44909,6 +45619,9 @@
       <c r="AV237" t="n">
         <v>-4.095137490646891</v>
       </c>
+      <c r="AW237" t="n">
+        <v>67.858169885379</v>
+      </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
@@ -45097,6 +45810,9 @@
       <c r="AV238" t="n">
         <v>-6.318255286702083</v>
       </c>
+      <c r="AW238" t="n">
+        <v>82.94787504798001</v>
+      </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
@@ -45283,6 +45999,9 @@
       <c r="AV239" t="n">
         <v>-4.095137490646891</v>
       </c>
+      <c r="AW239" t="n">
+        <v>67.858169885379</v>
+      </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
@@ -45469,6 +46188,9 @@
       <c r="AV240" t="n">
         <v>-4.095137490646891</v>
       </c>
+      <c r="AW240" t="n">
+        <v>67.858169885379</v>
+      </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
@@ -45655,6 +46377,9 @@
       <c r="AV241" t="n">
         <v>-10.94007065918665</v>
       </c>
+      <c r="AW241" t="n">
+        <v>119.17898068922</v>
+      </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
@@ -45841,6 +46566,9 @@
       <c r="AV242" t="n">
         <v>-4.095137490646891</v>
       </c>
+      <c r="AW242" t="n">
+        <v>67.858169885379</v>
+      </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
@@ -46029,6 +46757,9 @@
       <c r="AV243" t="n">
         <v>-10.2969188737567</v>
       </c>
+      <c r="AW243" t="n">
+        <v>105.80010911054</v>
+      </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
@@ -46215,6 +46946,9 @@
       <c r="AV244" t="n">
         <v>-4.095137490646891</v>
       </c>
+      <c r="AW244" t="n">
+        <v>67.858169885379</v>
+      </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
@@ -46403,6 +47137,9 @@
       <c r="AV245" t="n">
         <v>-10.2969188737567</v>
       </c>
+      <c r="AW245" t="n">
+        <v>105.80010911054</v>
+      </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
@@ -46591,6 +47328,9 @@
       <c r="AV246" t="n">
         <v>-8.868221210463872</v>
       </c>
+      <c r="AW246" t="n">
+        <v>154.28804453106</v>
+      </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
@@ -46779,6 +47519,9 @@
       <c r="AV247" t="n">
         <v>-2.005337503537632</v>
       </c>
+      <c r="AW247" t="n">
+        <v>40.311887445036</v>
+      </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
@@ -46967,6 +47710,9 @@
       <c r="AV248" t="n">
         <v>-6.318255286702083</v>
       </c>
+      <c r="AW248" t="n">
+        <v>82.94787504798001</v>
+      </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
@@ -47155,6 +47901,9 @@
       <c r="AV249" t="n">
         <v>-10.2969188737567</v>
       </c>
+      <c r="AW249" t="n">
+        <v>105.80010911054</v>
+      </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
@@ -47343,6 +48092,9 @@
       <c r="AV250" t="n">
         <v>-7.44064593044142</v>
       </c>
+      <c r="AW250" t="n">
+        <v>114.8530178201</v>
+      </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
@@ -47531,6 +48283,9 @@
       <c r="AV251" t="n">
         <v>-4.095137490646891</v>
       </c>
+      <c r="AW251" t="n">
+        <v>67.858169885379</v>
+      </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
@@ -47719,6 +48474,9 @@
       <c r="AV252" t="n">
         <v>-6.318255286702083</v>
       </c>
+      <c r="AW252" t="n">
+        <v>82.94787504798001</v>
+      </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
@@ -47905,6 +48663,9 @@
       <c r="AV253" t="n">
         <v>-4.095137490646891</v>
       </c>
+      <c r="AW253" t="n">
+        <v>67.858169885379</v>
+      </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
@@ -48093,6 +48854,9 @@
       <c r="AV254" t="n">
         <v>-10.2969188737567</v>
       </c>
+      <c r="AW254" t="n">
+        <v>105.80010911054</v>
+      </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
@@ -48279,6 +49043,9 @@
       <c r="AV255" t="n">
         <v>-4.095137490646891</v>
       </c>
+      <c r="AW255" t="n">
+        <v>67.858169885379</v>
+      </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
@@ -48465,6 +49232,9 @@
       <c r="AV256" t="n">
         <v>-10.2969188737567</v>
       </c>
+      <c r="AW256" t="n">
+        <v>105.80010911054</v>
+      </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
@@ -48651,6 +49421,9 @@
       <c r="AV257" t="n">
         <v>-10.2969188737567</v>
       </c>
+      <c r="AW257" t="n">
+        <v>105.80010911054</v>
+      </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
@@ -48837,6 +49610,9 @@
       <c r="AV258" t="n">
         <v>-10.2969188737567</v>
       </c>
+      <c r="AW258" t="n">
+        <v>105.80010911054</v>
+      </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
@@ -49023,6 +49799,9 @@
       <c r="AV259" t="n">
         <v>8.931062066007797</v>
       </c>
+      <c r="AW259" t="n">
+        <v>145.73468991087</v>
+      </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
@@ -49211,6 +49990,9 @@
       <c r="AV260" t="n">
         <v>3.908686776894172</v>
       </c>
+      <c r="AW260" t="n">
+        <v>41.64119215621</v>
+      </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
@@ -49397,6 +50179,9 @@
       <c r="AV261" t="n">
         <v>6.882337865903551</v>
       </c>
+      <c r="AW261" t="n">
+        <v>113.08790347101</v>
+      </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
@@ -49585,6 +50370,9 @@
       <c r="AV262" t="n">
         <v>6.683144185002803</v>
       </c>
+      <c r="AW262" t="n">
+        <v>115.59391415764</v>
+      </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
@@ -49773,6 +50561,9 @@
       <c r="AV263" t="n">
         <v>3.669999861567348</v>
       </c>
+      <c r="AW263" t="n">
+        <v>67.878829091028</v>
+      </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
@@ -49961,6 +50752,9 @@
       <c r="AV264" t="n">
         <v>5.937508573074396</v>
       </c>
+      <c r="AW264" t="n">
+        <v>36.833662831508</v>
+      </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
@@ -50147,6 +50941,9 @@
       <c r="AV265" t="n">
         <v>6.683144185002803</v>
       </c>
+      <c r="AW265" t="n">
+        <v>115.59391415764</v>
+      </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
@@ -50335,6 +51132,9 @@
       <c r="AV266" t="n">
         <v>8.575950904856498</v>
       </c>
+      <c r="AW266" t="n">
+        <v>105.19601117124</v>
+      </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
@@ -50523,6 +51323,9 @@
       <c r="AV267" t="n">
         <v>4.795329105514583</v>
       </c>
+      <c r="AW267" t="n">
+        <v>82.490091091384</v>
+      </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
@@ -50711,6 +51514,9 @@
       <c r="AV268" t="n">
         <v>5.937508573074396</v>
       </c>
+      <c r="AW268" t="n">
+        <v>36.833662831508</v>
+      </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
@@ -50899,6 +51705,9 @@
       <c r="AV269" t="n">
         <v>8.575950904856498</v>
       </c>
+      <c r="AW269" t="n">
+        <v>105.19601117124</v>
+      </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
@@ -51087,6 +51896,9 @@
       <c r="AV270" t="n">
         <v>5.937508573074396</v>
       </c>
+      <c r="AW270" t="n">
+        <v>36.833662831508</v>
+      </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
@@ -51291,6 +52103,9 @@
       <c r="AV271" t="n">
         <v>6.202554015860812</v>
       </c>
+      <c r="AW271" t="n">
+        <v>107.9352519968</v>
+      </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
@@ -51477,6 +52292,9 @@
       <c r="AV272" t="n">
         <v>3.669999861567348</v>
       </c>
+      <c r="AW272" t="n">
+        <v>67.878829091028</v>
+      </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
@@ -51665,6 +52483,9 @@
       <c r="AV273" t="n">
         <v>6.276830732305257</v>
       </c>
+      <c r="AW273" t="n">
+        <v>50.43564578543</v>
+      </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
@@ -51853,6 +52674,9 @@
       <c r="AV274" t="n">
         <v>6.683144185002803</v>
       </c>
+      <c r="AW274" t="n">
+        <v>115.59391415764</v>
+      </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
@@ -52042,6 +52866,9 @@
       <c r="AV275" t="n">
         <v>6.276830732305257</v>
       </c>
+      <c r="AW275" t="n">
+        <v>50.43564578543</v>
+      </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
@@ -52228,6 +53055,9 @@
       <c r="AV276" t="n">
         <v>5.391888041414731</v>
       </c>
+      <c r="AW276" t="n">
+        <v>40.980865664706</v>
+      </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
@@ -52416,6 +53246,9 @@
       <c r="AV277" t="n">
         <v>8.931062066007797</v>
       </c>
+      <c r="AW277" t="n">
+        <v>145.73468991087</v>
+      </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
@@ -52603,6 +53436,9 @@
       <c r="AV278" t="n">
         <v>8.575950904856498</v>
       </c>
+      <c r="AW278" t="n">
+        <v>105.19601117124</v>
+      </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
@@ -52791,6 +53627,9 @@
       <c r="AV279" t="n">
         <v>5.937508573074396</v>
       </c>
+      <c r="AW279" t="n">
+        <v>36.833662831508</v>
+      </c>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
@@ -52980,6 +53819,9 @@
       <c r="AV280" t="n">
         <v>3.669999861567348</v>
       </c>
+      <c r="AW280" t="n">
+        <v>67.878829091028</v>
+      </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
@@ -53168,6 +54010,9 @@
       <c r="AV281" t="n">
         <v>6.276830732305257</v>
       </c>
+      <c r="AW281" t="n">
+        <v>50.43564578543</v>
+      </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
@@ -53356,6 +54201,9 @@
       <c r="AV282" t="n">
         <v>5.391888041414731</v>
       </c>
+      <c r="AW282" t="n">
+        <v>40.980865664706</v>
+      </c>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
@@ -53542,6 +54390,9 @@
       <c r="AV283" t="n">
         <v>3.669999861567348</v>
       </c>
+      <c r="AW283" t="n">
+        <v>67.878829091028</v>
+      </c>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
@@ -53730,6 +54581,9 @@
       <c r="AV284" t="n">
         <v>8.575950904856498</v>
       </c>
+      <c r="AW284" t="n">
+        <v>105.19601117124</v>
+      </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
@@ -53918,6 +54772,9 @@
       <c r="AV285" t="n">
         <v>8.931062066007797</v>
       </c>
+      <c r="AW285" t="n">
+        <v>145.73468991087</v>
+      </c>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
@@ -54104,6 +54961,9 @@
       <c r="AV286" t="n">
         <v>5.391888041414731</v>
       </c>
+      <c r="AW286" t="n">
+        <v>40.980865664706</v>
+      </c>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
@@ -54290,6 +55150,9 @@
       <c r="AV287" t="n">
         <v>6.276830732305257</v>
       </c>
+      <c r="AW287" t="n">
+        <v>50.43564578543</v>
+      </c>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
@@ -54476,6 +55339,9 @@
       <c r="AV288" t="n">
         <v>6.276830732305257</v>
       </c>
+      <c r="AW288" t="n">
+        <v>50.43564578543</v>
+      </c>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
@@ -54680,6 +55546,9 @@
       <c r="AV289" t="n">
         <v>5.391888041414731</v>
       </c>
+      <c r="AW289" t="n">
+        <v>40.980865664706</v>
+      </c>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
@@ -54866,6 +55735,9 @@
       <c r="AV290" t="n">
         <v>8.575950904856498</v>
       </c>
+      <c r="AW290" t="n">
+        <v>105.19601117124</v>
+      </c>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
@@ -55054,6 +55926,9 @@
       <c r="AV291" t="n">
         <v>1.459288507572694</v>
       </c>
+      <c r="AW291" t="n">
+        <v>33.752971546974</v>
+      </c>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
@@ -55242,6 +56117,9 @@
       <c r="AV292" t="n">
         <v>4.839085147144033</v>
       </c>
+      <c r="AW292" t="n">
+        <v>100.43232570399</v>
+      </c>
     </row>
     <row r="293">
       <c r="A293" t="inlineStr">
@@ -55428,6 +56306,9 @@
       <c r="AV293" t="n">
         <v>4.839085147144033</v>
       </c>
+      <c r="AW293" t="n">
+        <v>100.43232570399</v>
+      </c>
     </row>
     <row r="294">
       <c r="A294" t="inlineStr">
@@ -55616,6 +56497,9 @@
       <c r="AV294" t="n">
         <v>8.619503551914917</v>
       </c>
+      <c r="AW294" t="n">
+        <v>43.143073237403</v>
+      </c>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
@@ -55804,6 +56688,9 @@
       <c r="AV295" t="n">
         <v>6.179312225729632</v>
       </c>
+      <c r="AW295" t="n">
+        <v>109.40393002769</v>
+      </c>
     </row>
     <row r="296">
       <c r="A296" t="inlineStr">
@@ -55992,6 +56879,9 @@
       <c r="AV296" t="n">
         <v>3.005635160762978</v>
       </c>
+      <c r="AW296" t="n">
+        <v>36.270510219437</v>
+      </c>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
@@ -56180,6 +57070,9 @@
       <c r="AV297" t="n">
         <v>4.839085147144033</v>
       </c>
+      <c r="AW297" t="n">
+        <v>100.43232570399</v>
+      </c>
     </row>
     <row r="298">
       <c r="A298" t="inlineStr">
@@ -56369,6 +57262,9 @@
       <c r="AV298" t="n">
         <v>2.570840474439692</v>
       </c>
+      <c r="AW298" t="n">
+        <v>111.95130179017</v>
+      </c>
     </row>
     <row r="299">
       <c r="A299" t="inlineStr">
@@ -56558,6 +57454,9 @@
       <c r="AV299" t="n">
         <v>1.459288507572694</v>
       </c>
+      <c r="AW299" t="n">
+        <v>33.752971546974</v>
+      </c>
     </row>
     <row r="300">
       <c r="A300" t="inlineStr">
@@ -56746,6 +57645,9 @@
       <c r="AV300" t="n">
         <v>1.459288507572694</v>
       </c>
+      <c r="AW300" t="n">
+        <v>33.752971546974</v>
+      </c>
     </row>
     <row r="301">
       <c r="A301" t="inlineStr">
@@ -56933,6 +57835,9 @@
       <c r="AV301" t="n">
         <v>2.570840474439692</v>
       </c>
+      <c r="AW301" t="n">
+        <v>111.95130179017</v>
+      </c>
     </row>
     <row r="302">
       <c r="A302" t="inlineStr">
@@ -57121,6 +58026,9 @@
       <c r="AV302" t="n">
         <v>4.839085147144033</v>
       </c>
+      <c r="AW302" t="n">
+        <v>100.43232570399</v>
+      </c>
     </row>
     <row r="303">
       <c r="A303" t="inlineStr">
@@ -57309,6 +58217,9 @@
       <c r="AV303" t="n">
         <v>8.619503551914917</v>
       </c>
+      <c r="AW303" t="n">
+        <v>43.143073237403</v>
+      </c>
     </row>
     <row r="304">
       <c r="A304" t="inlineStr">
@@ -57495,6 +58406,9 @@
       <c r="AV304" t="n">
         <v>2.568328178340693</v>
       </c>
+      <c r="AW304" t="n">
+        <v>37.194739974863</v>
+      </c>
     </row>
     <row r="305">
       <c r="A305" t="inlineStr">
@@ -57681,6 +58595,9 @@
       <c r="AV305" t="n">
         <v>2.568328178340693</v>
       </c>
+      <c r="AW305" t="n">
+        <v>37.194739974863</v>
+      </c>
     </row>
     <row r="306">
       <c r="A306" t="inlineStr">
@@ -57869,6 +58786,9 @@
       <c r="AV306" t="n">
         <v>4.233431833691697</v>
       </c>
+      <c r="AW306" t="n">
+        <v>104.28155910894</v>
+      </c>
     </row>
     <row r="307">
       <c r="A307" t="inlineStr">
@@ -58055,6 +58975,9 @@
       <c r="AV307" t="n">
         <v>5.007234590450366</v>
       </c>
+      <c r="AW307" t="n">
+        <v>48.353625405003</v>
+      </c>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">
@@ -58243,6 +59166,9 @@
       <c r="AV308" t="n">
         <v>1.459288507572694</v>
       </c>
+      <c r="AW308" t="n">
+        <v>33.752971546974</v>
+      </c>
     </row>
     <row r="309">
       <c r="A309" t="inlineStr">
@@ -58429,6 +59355,9 @@
       <c r="AV309" t="n">
         <v>1.459288507572694</v>
       </c>
+      <c r="AW309" t="n">
+        <v>33.752971546974</v>
+      </c>
     </row>
     <row r="310">
       <c r="A310" t="inlineStr">
@@ -58617,6 +59546,9 @@
       <c r="AV310" t="n">
         <v>1.369731055365847</v>
       </c>
+      <c r="AW310" t="n">
+        <v>64.78935720879601</v>
+      </c>
     </row>
     <row r="311">
       <c r="A311" t="inlineStr">
@@ -58805,6 +59737,9 @@
       <c r="AV311" t="n">
         <v>1.540173107095669</v>
       </c>
+      <c r="AW311" t="n">
+        <v>29.69814656209</v>
+      </c>
     </row>
     <row r="312">
       <c r="A312" t="inlineStr">
@@ -58993,6 +59928,9 @@
       <c r="AV312" t="n">
         <v>4.839085147144033</v>
       </c>
+      <c r="AW312" t="n">
+        <v>100.43232570399</v>
+      </c>
     </row>
     <row r="313">
       <c r="A313" t="inlineStr">
@@ -59179,6 +60117,9 @@
       <c r="AV313" t="n">
         <v>4.839085147144033</v>
       </c>
+      <c r="AW313" t="n">
+        <v>100.43232570399</v>
+      </c>
     </row>
     <row r="314">
       <c r="A314" t="inlineStr">
@@ -59368,6 +60309,9 @@
       <c r="AV314" t="n">
         <v>1.369731055365847</v>
       </c>
+      <c r="AW314" t="n">
+        <v>64.78935720879601</v>
+      </c>
     </row>
     <row r="315">
       <c r="A315" t="inlineStr">
@@ -59556,6 +60500,9 @@
       <c r="AV315" t="n">
         <v>2.570840474439692</v>
       </c>
+      <c r="AW315" t="n">
+        <v>111.95130179017</v>
+      </c>
     </row>
     <row r="316">
       <c r="A316" t="inlineStr">
@@ -59742,6 +60689,9 @@
       <c r="AV316" t="n">
         <v>5.007234590450366</v>
       </c>
+      <c r="AW316" t="n">
+        <v>48.353625405003</v>
+      </c>
     </row>
     <row r="317">
       <c r="A317" t="inlineStr">
@@ -59930,6 +60880,9 @@
       <c r="AV317" t="n">
         <v>8.619503551914917</v>
       </c>
+      <c r="AW317" t="n">
+        <v>43.143073237403</v>
+      </c>
     </row>
     <row r="318">
       <c r="A318" t="inlineStr">
@@ -60118,6 +61071,9 @@
       <c r="AV318" t="n">
         <v>0.3399661580034632</v>
       </c>
+      <c r="AW318" t="n">
+        <v>101.14707428399</v>
+      </c>
     </row>
     <row r="319">
       <c r="A319" t="inlineStr">
@@ -60323,6 +61279,9 @@
       <c r="AV319" t="n">
         <v>-0.3106701847258933</v>
       </c>
+      <c r="AW319" t="n">
+        <v>36.37122985845</v>
+      </c>
     </row>
     <row r="320">
       <c r="A320" t="inlineStr">
@@ -60511,6 +61470,9 @@
       <c r="AV320" t="n">
         <v>0.3399661580034632</v>
       </c>
+      <c r="AW320" t="n">
+        <v>101.14707428399</v>
+      </c>
     </row>
     <row r="321">
       <c r="A321" t="inlineStr">
@@ -60699,6 +61661,9 @@
       <c r="AV321" t="n">
         <v>0.9364875026714827</v>
       </c>
+      <c r="AW321" t="n">
+        <v>110.6417894474</v>
+      </c>
     </row>
     <row r="322">
       <c r="A322" t="inlineStr">
@@ -60886,6 +61851,9 @@
       <c r="AV322" t="n">
         <v>0.9364875026714827</v>
       </c>
+      <c r="AW322" t="n">
+        <v>110.6417894474</v>
+      </c>
     </row>
     <row r="323">
       <c r="A323" t="inlineStr">
@@ -61074,6 +62042,9 @@
       <c r="AV323" t="n">
         <v>0.07456072164949035</v>
       </c>
+      <c r="AW323" t="n">
+        <v>45.023552850836</v>
+      </c>
     </row>
     <row r="324">
       <c r="A324" t="inlineStr">
@@ -61260,6 +62231,9 @@
       <c r="AV324" t="n">
         <v>0.07456072164949035</v>
       </c>
+      <c r="AW324" t="n">
+        <v>45.023552850836</v>
+      </c>
     </row>
     <row r="325">
       <c r="A325" t="inlineStr">
@@ -61446,6 +62420,9 @@
       <c r="AV325" t="n">
         <v>0.9364875026714827</v>
       </c>
+      <c r="AW325" t="n">
+        <v>110.6417894474</v>
+      </c>
     </row>
     <row r="326">
       <c r="A326" t="inlineStr">
@@ -61634,6 +62611,9 @@
       <c r="AV326" t="n">
         <v>1.251700632035949</v>
       </c>
+      <c r="AW326" t="n">
+        <v>105.17086569329</v>
+      </c>
     </row>
     <row r="327">
       <c r="A327" t="inlineStr">
@@ -61821,6 +62801,9 @@
       </c>
       <c r="AV327" t="n">
         <v>-0.3106701847258933</v>
+      </c>
+      <c r="AW327" t="n">
+        <v>36.37122985845</v>
       </c>
     </row>
   </sheetData>

</xml_diff>